<commit_message>
BF additions and Zim calibration
</commit_message>
<xml_diff>
--- a/my_countries/ZIM/outputs/zim-sim_default_scenario_A.xlsx
+++ b/my_countries/ZIM/outputs/zim-sim_default_scenario_A.xlsx
@@ -811,7 +811,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AK206"/>
+  <dimension ref="A1:AK167"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -19664,4296 +19664,6 @@
         <v>0</v>
       </c>
       <c r="AK167">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="168" spans="1:37">
-      <c r="A168" s="2">
-        <v>44076</v>
-      </c>
-      <c r="B168">
-        <v>166</v>
-      </c>
-      <c r="C168">
-        <v>1137715.655858824</v>
-      </c>
-      <c r="D168">
-        <v>1138183.442082663</v>
-      </c>
-      <c r="E168">
-        <v>0</v>
-      </c>
-      <c r="F168">
-        <v>0</v>
-      </c>
-      <c r="G168">
-        <v>1135977.261351267</v>
-      </c>
-      <c r="H168">
-        <v>690670.0257366077</v>
-      </c>
-      <c r="I168">
-        <v>24237.2503426687</v>
-      </c>
-      <c r="J168">
-        <v>5105.730586805043</v>
-      </c>
-      <c r="K168">
-        <v>1818.5831808</v>
-      </c>
-      <c r="L168">
-        <v>0</v>
-      </c>
-      <c r="M168">
-        <v>0</v>
-      </c>
-      <c r="N168">
-        <v>0</v>
-      </c>
-      <c r="O168">
-        <v>0</v>
-      </c>
-      <c r="P168">
-        <v>0</v>
-      </c>
-      <c r="Q168">
-        <v>45.00000000000001</v>
-      </c>
-      <c r="R168">
-        <v>15</v>
-      </c>
-      <c r="S168">
-        <v>0</v>
-      </c>
-      <c r="T168">
-        <v>0</v>
-      </c>
-      <c r="U168">
-        <v>0</v>
-      </c>
-      <c r="V168">
-        <v>0</v>
-      </c>
-      <c r="W168">
-        <v>362054.1554679333</v>
-      </c>
-      <c r="X168">
-        <v>150</v>
-      </c>
-      <c r="Y168">
-        <v>135</v>
-      </c>
-      <c r="Z168">
-        <v>105</v>
-      </c>
-      <c r="AA168">
-        <v>0</v>
-      </c>
-      <c r="AB168">
-        <v>0</v>
-      </c>
-      <c r="AC168">
-        <v>0</v>
-      </c>
-      <c r="AD168">
-        <v>0</v>
-      </c>
-      <c r="AE168">
-        <v>1498181.4168192</v>
-      </c>
-      <c r="AF168">
-        <v>0.0001001213860458009</v>
-      </c>
-      <c r="AG168">
-        <v>0</v>
-      </c>
-      <c r="AH168">
-        <v>0</v>
-      </c>
-      <c r="AJ168">
-        <v>0</v>
-      </c>
-      <c r="AK168">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="169" spans="1:37">
-      <c r="A169" s="2">
-        <v>44077</v>
-      </c>
-      <c r="B169">
-        <v>167</v>
-      </c>
-      <c r="C169">
-        <v>1137715.655858824</v>
-      </c>
-      <c r="D169">
-        <v>1138183.442082663</v>
-      </c>
-      <c r="E169">
-        <v>0</v>
-      </c>
-      <c r="F169">
-        <v>0</v>
-      </c>
-      <c r="G169">
-        <v>1135977.261351267</v>
-      </c>
-      <c r="H169">
-        <v>690670.0257366077</v>
-      </c>
-      <c r="I169">
-        <v>24237.2503426687</v>
-      </c>
-      <c r="J169">
-        <v>5105.730586805043</v>
-      </c>
-      <c r="K169">
-        <v>1818.5831808</v>
-      </c>
-      <c r="L169">
-        <v>0</v>
-      </c>
-      <c r="M169">
-        <v>0</v>
-      </c>
-      <c r="N169">
-        <v>0</v>
-      </c>
-      <c r="O169">
-        <v>0</v>
-      </c>
-      <c r="P169">
-        <v>0</v>
-      </c>
-      <c r="Q169">
-        <v>0</v>
-      </c>
-      <c r="R169">
-        <v>0</v>
-      </c>
-      <c r="S169">
-        <v>0</v>
-      </c>
-      <c r="T169">
-        <v>0</v>
-      </c>
-      <c r="U169">
-        <v>0</v>
-      </c>
-      <c r="V169">
-        <v>0</v>
-      </c>
-      <c r="W169">
-        <v>362054.1554679333</v>
-      </c>
-      <c r="X169">
-        <v>150</v>
-      </c>
-      <c r="Y169">
-        <v>135</v>
-      </c>
-      <c r="Z169">
-        <v>105</v>
-      </c>
-      <c r="AA169">
-        <v>0</v>
-      </c>
-      <c r="AB169">
-        <v>0</v>
-      </c>
-      <c r="AC169">
-        <v>0</v>
-      </c>
-      <c r="AD169">
-        <v>0</v>
-      </c>
-      <c r="AE169">
-        <v>1498181.4168192</v>
-      </c>
-      <c r="AF169">
-        <v>0.0001001213860458009</v>
-      </c>
-      <c r="AG169">
-        <v>0</v>
-      </c>
-      <c r="AH169">
-        <v>0</v>
-      </c>
-      <c r="AJ169">
-        <v>0</v>
-      </c>
-      <c r="AK169">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="170" spans="1:37">
-      <c r="A170" s="2">
-        <v>44078</v>
-      </c>
-      <c r="B170">
-        <v>168</v>
-      </c>
-      <c r="C170">
-        <v>1137715.655858824</v>
-      </c>
-      <c r="D170">
-        <v>1138198.442082663</v>
-      </c>
-      <c r="E170">
-        <v>0</v>
-      </c>
-      <c r="F170">
-        <v>0</v>
-      </c>
-      <c r="G170">
-        <v>1135992.261351267</v>
-      </c>
-      <c r="H170">
-        <v>690670.0257366077</v>
-      </c>
-      <c r="I170">
-        <v>24252.2503426687</v>
-      </c>
-      <c r="J170">
-        <v>5105.730586805043</v>
-      </c>
-      <c r="K170">
-        <v>1818.5831808</v>
-      </c>
-      <c r="L170">
-        <v>0</v>
-      </c>
-      <c r="M170">
-        <v>0</v>
-      </c>
-      <c r="N170">
-        <v>15</v>
-      </c>
-      <c r="O170">
-        <v>0</v>
-      </c>
-      <c r="P170">
-        <v>0</v>
-      </c>
-      <c r="Q170">
-        <v>15</v>
-      </c>
-      <c r="R170">
-        <v>0</v>
-      </c>
-      <c r="S170">
-        <v>15</v>
-      </c>
-      <c r="T170">
-        <v>0</v>
-      </c>
-      <c r="U170">
-        <v>0</v>
-      </c>
-      <c r="V170">
-        <v>0</v>
-      </c>
-      <c r="W170">
-        <v>362054.1554679333</v>
-      </c>
-      <c r="X170">
-        <v>135</v>
-      </c>
-      <c r="Y170">
-        <v>135</v>
-      </c>
-      <c r="Z170">
-        <v>105</v>
-      </c>
-      <c r="AA170">
-        <v>15</v>
-      </c>
-      <c r="AB170">
-        <v>0</v>
-      </c>
-      <c r="AC170">
-        <v>0</v>
-      </c>
-      <c r="AD170">
-        <v>0</v>
-      </c>
-      <c r="AE170">
-        <v>1498181.4168192</v>
-      </c>
-      <c r="AF170">
-        <v>9.010924744122079E-05</v>
-      </c>
-      <c r="AG170">
-        <v>0</v>
-      </c>
-      <c r="AH170">
-        <v>0</v>
-      </c>
-      <c r="AJ170">
-        <v>0</v>
-      </c>
-      <c r="AK170">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="171" spans="1:37">
-      <c r="A171" s="2">
-        <v>44079</v>
-      </c>
-      <c r="B171">
-        <v>169</v>
-      </c>
-      <c r="C171">
-        <v>1137715.655858824</v>
-      </c>
-      <c r="D171">
-        <v>1138198.442082663</v>
-      </c>
-      <c r="E171">
-        <v>0</v>
-      </c>
-      <c r="F171">
-        <v>0</v>
-      </c>
-      <c r="G171">
-        <v>1135992.261351267</v>
-      </c>
-      <c r="H171">
-        <v>690685.0257366077</v>
-      </c>
-      <c r="I171">
-        <v>24252.2503426687</v>
-      </c>
-      <c r="J171">
-        <v>5105.730586805043</v>
-      </c>
-      <c r="K171">
-        <v>1818.5831808</v>
-      </c>
-      <c r="L171">
-        <v>0</v>
-      </c>
-      <c r="M171">
-        <v>0</v>
-      </c>
-      <c r="N171">
-        <v>0</v>
-      </c>
-      <c r="O171">
-        <v>0</v>
-      </c>
-      <c r="P171">
-        <v>0</v>
-      </c>
-      <c r="Q171">
-        <v>0</v>
-      </c>
-      <c r="R171">
-        <v>15</v>
-      </c>
-      <c r="S171">
-        <v>0</v>
-      </c>
-      <c r="T171">
-        <v>0</v>
-      </c>
-      <c r="U171">
-        <v>0</v>
-      </c>
-      <c r="V171">
-        <v>0</v>
-      </c>
-      <c r="W171">
-        <v>362054.1554679333</v>
-      </c>
-      <c r="X171">
-        <v>135</v>
-      </c>
-      <c r="Y171">
-        <v>135</v>
-      </c>
-      <c r="Z171">
-        <v>120</v>
-      </c>
-      <c r="AA171">
-        <v>15</v>
-      </c>
-      <c r="AB171">
-        <v>0</v>
-      </c>
-      <c r="AC171">
-        <v>0</v>
-      </c>
-      <c r="AD171">
-        <v>0</v>
-      </c>
-      <c r="AE171">
-        <v>1498181.4168192</v>
-      </c>
-      <c r="AF171">
-        <v>9.010924744122079E-05</v>
-      </c>
-      <c r="AG171">
-        <v>0</v>
-      </c>
-      <c r="AH171">
-        <v>0</v>
-      </c>
-      <c r="AJ171">
-        <v>0</v>
-      </c>
-      <c r="AK171">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="172" spans="1:37">
-      <c r="A172" s="2">
-        <v>44080</v>
-      </c>
-      <c r="B172">
-        <v>170</v>
-      </c>
-      <c r="C172">
-        <v>1137715.655858824</v>
-      </c>
-      <c r="D172">
-        <v>1138198.442082663</v>
-      </c>
-      <c r="E172">
-        <v>0</v>
-      </c>
-      <c r="F172">
-        <v>0</v>
-      </c>
-      <c r="G172">
-        <v>1136037.261351267</v>
-      </c>
-      <c r="H172">
-        <v>690685.0257366077</v>
-      </c>
-      <c r="I172">
-        <v>24252.2503426687</v>
-      </c>
-      <c r="J172">
-        <v>5105.730586805043</v>
-      </c>
-      <c r="K172">
-        <v>1818.5831808</v>
-      </c>
-      <c r="L172">
-        <v>0</v>
-      </c>
-      <c r="M172">
-        <v>0</v>
-      </c>
-      <c r="N172">
-        <v>0</v>
-      </c>
-      <c r="O172">
-        <v>0</v>
-      </c>
-      <c r="P172">
-        <v>0</v>
-      </c>
-      <c r="Q172">
-        <v>45.00000000000001</v>
-      </c>
-      <c r="R172">
-        <v>0</v>
-      </c>
-      <c r="S172">
-        <v>0</v>
-      </c>
-      <c r="T172">
-        <v>0</v>
-      </c>
-      <c r="U172">
-        <v>0</v>
-      </c>
-      <c r="V172">
-        <v>0</v>
-      </c>
-      <c r="W172">
-        <v>362054.1554679333</v>
-      </c>
-      <c r="X172">
-        <v>90.00000000000001</v>
-      </c>
-      <c r="Y172">
-        <v>90.00000000000001</v>
-      </c>
-      <c r="Z172">
-        <v>75.00000000000001</v>
-      </c>
-      <c r="AA172">
-        <v>15</v>
-      </c>
-      <c r="AB172">
-        <v>0</v>
-      </c>
-      <c r="AC172">
-        <v>0</v>
-      </c>
-      <c r="AD172">
-        <v>0</v>
-      </c>
-      <c r="AE172">
-        <v>1498181.4168192</v>
-      </c>
-      <c r="AF172">
-        <v>6.007283162748053E-05</v>
-      </c>
-      <c r="AG172">
-        <v>0</v>
-      </c>
-      <c r="AH172">
-        <v>0</v>
-      </c>
-      <c r="AJ172">
-        <v>0</v>
-      </c>
-      <c r="AK172">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="173" spans="1:37">
-      <c r="A173" s="2">
-        <v>44081</v>
-      </c>
-      <c r="B173">
-        <v>171</v>
-      </c>
-      <c r="C173">
-        <v>1137715.655858824</v>
-      </c>
-      <c r="D173">
-        <v>1138198.442082663</v>
-      </c>
-      <c r="E173">
-        <v>0</v>
-      </c>
-      <c r="F173">
-        <v>0</v>
-      </c>
-      <c r="G173">
-        <v>1136052.261351267</v>
-      </c>
-      <c r="H173">
-        <v>690685.0257366077</v>
-      </c>
-      <c r="I173">
-        <v>24252.2503426687</v>
-      </c>
-      <c r="J173">
-        <v>5105.730586805043</v>
-      </c>
-      <c r="K173">
-        <v>1818.5831808</v>
-      </c>
-      <c r="L173">
-        <v>0</v>
-      </c>
-      <c r="M173">
-        <v>0</v>
-      </c>
-      <c r="N173">
-        <v>0</v>
-      </c>
-      <c r="O173">
-        <v>0</v>
-      </c>
-      <c r="P173">
-        <v>0</v>
-      </c>
-      <c r="Q173">
-        <v>15</v>
-      </c>
-      <c r="R173">
-        <v>0</v>
-      </c>
-      <c r="S173">
-        <v>0</v>
-      </c>
-      <c r="T173">
-        <v>0</v>
-      </c>
-      <c r="U173">
-        <v>0</v>
-      </c>
-      <c r="V173">
-        <v>0</v>
-      </c>
-      <c r="W173">
-        <v>362054.1554679333</v>
-      </c>
-      <c r="X173">
-        <v>75.00000000000001</v>
-      </c>
-      <c r="Y173">
-        <v>75.00000000000001</v>
-      </c>
-      <c r="Z173">
-        <v>60.00000000000001</v>
-      </c>
-      <c r="AA173">
-        <v>15</v>
-      </c>
-      <c r="AB173">
-        <v>0</v>
-      </c>
-      <c r="AC173">
-        <v>0</v>
-      </c>
-      <c r="AD173">
-        <v>0</v>
-      </c>
-      <c r="AE173">
-        <v>1498181.4168192</v>
-      </c>
-      <c r="AF173">
-        <v>5.006069302290044E-05</v>
-      </c>
-      <c r="AG173">
-        <v>0</v>
-      </c>
-      <c r="AH173">
-        <v>0</v>
-      </c>
-      <c r="AJ173">
-        <v>0</v>
-      </c>
-      <c r="AK173">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="174" spans="1:37">
-      <c r="A174" s="2">
-        <v>44082</v>
-      </c>
-      <c r="B174">
-        <v>172</v>
-      </c>
-      <c r="C174">
-        <v>1137715.655858824</v>
-      </c>
-      <c r="D174">
-        <v>1138198.442082663</v>
-      </c>
-      <c r="E174">
-        <v>0</v>
-      </c>
-      <c r="F174">
-        <v>0</v>
-      </c>
-      <c r="G174">
-        <v>1136082.261351267</v>
-      </c>
-      <c r="H174">
-        <v>690685.0257366077</v>
-      </c>
-      <c r="I174">
-        <v>24252.2503426687</v>
-      </c>
-      <c r="J174">
-        <v>5105.730586805043</v>
-      </c>
-      <c r="K174">
-        <v>1818.5831808</v>
-      </c>
-      <c r="L174">
-        <v>0</v>
-      </c>
-      <c r="M174">
-        <v>0</v>
-      </c>
-      <c r="N174">
-        <v>0</v>
-      </c>
-      <c r="O174">
-        <v>0</v>
-      </c>
-      <c r="P174">
-        <v>0</v>
-      </c>
-      <c r="Q174">
-        <v>30</v>
-      </c>
-      <c r="R174">
-        <v>0</v>
-      </c>
-      <c r="S174">
-        <v>0</v>
-      </c>
-      <c r="T174">
-        <v>0</v>
-      </c>
-      <c r="U174">
-        <v>0</v>
-      </c>
-      <c r="V174">
-        <v>0</v>
-      </c>
-      <c r="W174">
-        <v>362054.1554679333</v>
-      </c>
-      <c r="X174">
-        <v>45.00000000000001</v>
-      </c>
-      <c r="Y174">
-        <v>45.00000000000001</v>
-      </c>
-      <c r="Z174">
-        <v>45.00000000000001</v>
-      </c>
-      <c r="AA174">
-        <v>15</v>
-      </c>
-      <c r="AB174">
-        <v>0</v>
-      </c>
-      <c r="AC174">
-        <v>0</v>
-      </c>
-      <c r="AD174">
-        <v>0</v>
-      </c>
-      <c r="AE174">
-        <v>1498181.4168192</v>
-      </c>
-      <c r="AF174">
-        <v>3.003641581374026E-05</v>
-      </c>
-      <c r="AG174">
-        <v>0</v>
-      </c>
-      <c r="AH174">
-        <v>0</v>
-      </c>
-      <c r="AJ174">
-        <v>0</v>
-      </c>
-      <c r="AK174">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="175" spans="1:37">
-      <c r="A175" s="2">
-        <v>44083</v>
-      </c>
-      <c r="B175">
-        <v>173</v>
-      </c>
-      <c r="C175">
-        <v>1137715.655858824</v>
-      </c>
-      <c r="D175">
-        <v>1138198.442082663</v>
-      </c>
-      <c r="E175">
-        <v>0</v>
-      </c>
-      <c r="F175">
-        <v>0</v>
-      </c>
-      <c r="G175">
-        <v>1136082.261351267</v>
-      </c>
-      <c r="H175">
-        <v>690685.0257366077</v>
-      </c>
-      <c r="I175">
-        <v>24252.2503426687</v>
-      </c>
-      <c r="J175">
-        <v>5105.730586805043</v>
-      </c>
-      <c r="K175">
-        <v>1818.5831808</v>
-      </c>
-      <c r="L175">
-        <v>0</v>
-      </c>
-      <c r="M175">
-        <v>0</v>
-      </c>
-      <c r="N175">
-        <v>0</v>
-      </c>
-      <c r="O175">
-        <v>0</v>
-      </c>
-      <c r="P175">
-        <v>0</v>
-      </c>
-      <c r="Q175">
-        <v>0</v>
-      </c>
-      <c r="R175">
-        <v>0</v>
-      </c>
-      <c r="S175">
-        <v>0</v>
-      </c>
-      <c r="T175">
-        <v>0</v>
-      </c>
-      <c r="U175">
-        <v>0</v>
-      </c>
-      <c r="V175">
-        <v>0</v>
-      </c>
-      <c r="W175">
-        <v>362054.1554679333</v>
-      </c>
-      <c r="X175">
-        <v>45.00000000000001</v>
-      </c>
-      <c r="Y175">
-        <v>45.00000000000001</v>
-      </c>
-      <c r="Z175">
-        <v>45.00000000000001</v>
-      </c>
-      <c r="AA175">
-        <v>15</v>
-      </c>
-      <c r="AB175">
-        <v>0</v>
-      </c>
-      <c r="AC175">
-        <v>0</v>
-      </c>
-      <c r="AD175">
-        <v>0</v>
-      </c>
-      <c r="AE175">
-        <v>1498181.4168192</v>
-      </c>
-      <c r="AF175">
-        <v>3.003641581374026E-05</v>
-      </c>
-      <c r="AG175">
-        <v>0</v>
-      </c>
-      <c r="AH175">
-        <v>0</v>
-      </c>
-      <c r="AJ175">
-        <v>0</v>
-      </c>
-      <c r="AK175">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="176" spans="1:37">
-      <c r="A176" s="2">
-        <v>44084</v>
-      </c>
-      <c r="B176">
-        <v>174</v>
-      </c>
-      <c r="C176">
-        <v>1137715.655858824</v>
-      </c>
-      <c r="D176">
-        <v>1138198.442082663</v>
-      </c>
-      <c r="E176">
-        <v>0</v>
-      </c>
-      <c r="F176">
-        <v>0</v>
-      </c>
-      <c r="G176">
-        <v>1136082.261351267</v>
-      </c>
-      <c r="H176">
-        <v>690685.0257366077</v>
-      </c>
-      <c r="I176">
-        <v>24252.2503426687</v>
-      </c>
-      <c r="J176">
-        <v>5105.730586805043</v>
-      </c>
-      <c r="K176">
-        <v>1818.5831808</v>
-      </c>
-      <c r="L176">
-        <v>0</v>
-      </c>
-      <c r="M176">
-        <v>0</v>
-      </c>
-      <c r="N176">
-        <v>0</v>
-      </c>
-      <c r="O176">
-        <v>0</v>
-      </c>
-      <c r="P176">
-        <v>0</v>
-      </c>
-      <c r="Q176">
-        <v>0</v>
-      </c>
-      <c r="R176">
-        <v>0</v>
-      </c>
-      <c r="S176">
-        <v>0</v>
-      </c>
-      <c r="T176">
-        <v>0</v>
-      </c>
-      <c r="U176">
-        <v>0</v>
-      </c>
-      <c r="V176">
-        <v>0</v>
-      </c>
-      <c r="W176">
-        <v>362054.1554679333</v>
-      </c>
-      <c r="X176">
-        <v>45.00000000000001</v>
-      </c>
-      <c r="Y176">
-        <v>45.00000000000001</v>
-      </c>
-      <c r="Z176">
-        <v>45.00000000000001</v>
-      </c>
-      <c r="AA176">
-        <v>15</v>
-      </c>
-      <c r="AB176">
-        <v>0</v>
-      </c>
-      <c r="AC176">
-        <v>0</v>
-      </c>
-      <c r="AD176">
-        <v>0</v>
-      </c>
-      <c r="AE176">
-        <v>1498181.4168192</v>
-      </c>
-      <c r="AF176">
-        <v>3.003641581374026E-05</v>
-      </c>
-      <c r="AG176">
-        <v>0</v>
-      </c>
-      <c r="AH176">
-        <v>0</v>
-      </c>
-      <c r="AJ176">
-        <v>0</v>
-      </c>
-      <c r="AK176">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="177" spans="1:37">
-      <c r="A177" s="2">
-        <v>44085</v>
-      </c>
-      <c r="B177">
-        <v>175</v>
-      </c>
-      <c r="C177">
-        <v>1137715.655858824</v>
-      </c>
-      <c r="D177">
-        <v>1138198.442082663</v>
-      </c>
-      <c r="E177">
-        <v>0</v>
-      </c>
-      <c r="F177">
-        <v>0</v>
-      </c>
-      <c r="G177">
-        <v>1136082.261351267</v>
-      </c>
-      <c r="H177">
-        <v>690685.0257366077</v>
-      </c>
-      <c r="I177">
-        <v>24252.2503426687</v>
-      </c>
-      <c r="J177">
-        <v>5105.730586805043</v>
-      </c>
-      <c r="K177">
-        <v>1818.5831808</v>
-      </c>
-      <c r="L177">
-        <v>0</v>
-      </c>
-      <c r="M177">
-        <v>0</v>
-      </c>
-      <c r="N177">
-        <v>0</v>
-      </c>
-      <c r="O177">
-        <v>0</v>
-      </c>
-      <c r="P177">
-        <v>0</v>
-      </c>
-      <c r="Q177">
-        <v>0</v>
-      </c>
-      <c r="R177">
-        <v>0</v>
-      </c>
-      <c r="S177">
-        <v>0</v>
-      </c>
-      <c r="T177">
-        <v>0</v>
-      </c>
-      <c r="U177">
-        <v>0</v>
-      </c>
-      <c r="V177">
-        <v>0</v>
-      </c>
-      <c r="W177">
-        <v>362054.1554679333</v>
-      </c>
-      <c r="X177">
-        <v>45.00000000000001</v>
-      </c>
-      <c r="Y177">
-        <v>45.00000000000001</v>
-      </c>
-      <c r="Z177">
-        <v>45.00000000000001</v>
-      </c>
-      <c r="AA177">
-        <v>15</v>
-      </c>
-      <c r="AB177">
-        <v>0</v>
-      </c>
-      <c r="AC177">
-        <v>0</v>
-      </c>
-      <c r="AD177">
-        <v>0</v>
-      </c>
-      <c r="AE177">
-        <v>1498181.4168192</v>
-      </c>
-      <c r="AF177">
-        <v>3.003641581374026E-05</v>
-      </c>
-      <c r="AG177">
-        <v>0</v>
-      </c>
-      <c r="AH177">
-        <v>0</v>
-      </c>
-      <c r="AJ177">
-        <v>0</v>
-      </c>
-      <c r="AK177">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="178" spans="1:37">
-      <c r="A178" s="2">
-        <v>44086</v>
-      </c>
-      <c r="B178">
-        <v>176</v>
-      </c>
-      <c r="C178">
-        <v>1137715.655858824</v>
-      </c>
-      <c r="D178">
-        <v>1138198.442082663</v>
-      </c>
-      <c r="E178">
-        <v>0</v>
-      </c>
-      <c r="F178">
-        <v>0</v>
-      </c>
-      <c r="G178">
-        <v>1136097.261351267</v>
-      </c>
-      <c r="H178">
-        <v>690685.0257366077</v>
-      </c>
-      <c r="I178">
-        <v>24252.2503426687</v>
-      </c>
-      <c r="J178">
-        <v>5105.730586805043</v>
-      </c>
-      <c r="K178">
-        <v>1818.5831808</v>
-      </c>
-      <c r="L178">
-        <v>0</v>
-      </c>
-      <c r="M178">
-        <v>0</v>
-      </c>
-      <c r="N178">
-        <v>0</v>
-      </c>
-      <c r="O178">
-        <v>0</v>
-      </c>
-      <c r="P178">
-        <v>0</v>
-      </c>
-      <c r="Q178">
-        <v>15</v>
-      </c>
-      <c r="R178">
-        <v>0</v>
-      </c>
-      <c r="S178">
-        <v>0</v>
-      </c>
-      <c r="T178">
-        <v>0</v>
-      </c>
-      <c r="U178">
-        <v>0</v>
-      </c>
-      <c r="V178">
-        <v>0</v>
-      </c>
-      <c r="W178">
-        <v>362054.1554679333</v>
-      </c>
-      <c r="X178">
-        <v>30</v>
-      </c>
-      <c r="Y178">
-        <v>30</v>
-      </c>
-      <c r="Z178">
-        <v>30</v>
-      </c>
-      <c r="AA178">
-        <v>15</v>
-      </c>
-      <c r="AB178">
-        <v>0</v>
-      </c>
-      <c r="AC178">
-        <v>0</v>
-      </c>
-      <c r="AD178">
-        <v>0</v>
-      </c>
-      <c r="AE178">
-        <v>1498181.4168192</v>
-      </c>
-      <c r="AF178">
-        <v>2.002427720916017E-05</v>
-      </c>
-      <c r="AG178">
-        <v>0</v>
-      </c>
-      <c r="AH178">
-        <v>0</v>
-      </c>
-      <c r="AJ178">
-        <v>0</v>
-      </c>
-      <c r="AK178">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="179" spans="1:37">
-      <c r="A179" s="2">
-        <v>44087</v>
-      </c>
-      <c r="B179">
-        <v>177</v>
-      </c>
-      <c r="C179">
-        <v>1137715.655858824</v>
-      </c>
-      <c r="D179">
-        <v>1138198.442082663</v>
-      </c>
-      <c r="E179">
-        <v>0</v>
-      </c>
-      <c r="F179">
-        <v>0</v>
-      </c>
-      <c r="G179">
-        <v>1136112.261351267</v>
-      </c>
-      <c r="H179">
-        <v>690685.0257366077</v>
-      </c>
-      <c r="I179">
-        <v>24252.2503426687</v>
-      </c>
-      <c r="J179">
-        <v>5105.730586805043</v>
-      </c>
-      <c r="K179">
-        <v>1818.5831808</v>
-      </c>
-      <c r="L179">
-        <v>0</v>
-      </c>
-      <c r="M179">
-        <v>0</v>
-      </c>
-      <c r="N179">
-        <v>0</v>
-      </c>
-      <c r="O179">
-        <v>0</v>
-      </c>
-      <c r="P179">
-        <v>0</v>
-      </c>
-      <c r="Q179">
-        <v>15</v>
-      </c>
-      <c r="R179">
-        <v>0</v>
-      </c>
-      <c r="S179">
-        <v>0</v>
-      </c>
-      <c r="T179">
-        <v>0</v>
-      </c>
-      <c r="U179">
-        <v>0</v>
-      </c>
-      <c r="V179">
-        <v>0</v>
-      </c>
-      <c r="W179">
-        <v>362054.1554679333</v>
-      </c>
-      <c r="X179">
-        <v>15</v>
-      </c>
-      <c r="Y179">
-        <v>15</v>
-      </c>
-      <c r="Z179">
-        <v>15</v>
-      </c>
-      <c r="AA179">
-        <v>15</v>
-      </c>
-      <c r="AB179">
-        <v>0</v>
-      </c>
-      <c r="AC179">
-        <v>0</v>
-      </c>
-      <c r="AD179">
-        <v>0</v>
-      </c>
-      <c r="AE179">
-        <v>1498181.4168192</v>
-      </c>
-      <c r="AF179">
-        <v>1.001213860458009E-05</v>
-      </c>
-      <c r="AG179">
-        <v>0</v>
-      </c>
-      <c r="AH179">
-        <v>0</v>
-      </c>
-      <c r="AJ179">
-        <v>0</v>
-      </c>
-      <c r="AK179">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="180" spans="1:37">
-      <c r="A180" s="2">
-        <v>44088</v>
-      </c>
-      <c r="B180">
-        <v>178</v>
-      </c>
-      <c r="C180">
-        <v>1137715.655858824</v>
-      </c>
-      <c r="D180">
-        <v>1138198.442082663</v>
-      </c>
-      <c r="E180">
-        <v>0</v>
-      </c>
-      <c r="F180">
-        <v>0</v>
-      </c>
-      <c r="G180">
-        <v>1136112.261351267</v>
-      </c>
-      <c r="H180">
-        <v>690685.0257366077</v>
-      </c>
-      <c r="I180">
-        <v>24252.2503426687</v>
-      </c>
-      <c r="J180">
-        <v>5105.730586805043</v>
-      </c>
-      <c r="K180">
-        <v>1818.5831808</v>
-      </c>
-      <c r="L180">
-        <v>0</v>
-      </c>
-      <c r="M180">
-        <v>0</v>
-      </c>
-      <c r="N180">
-        <v>0</v>
-      </c>
-      <c r="O180">
-        <v>0</v>
-      </c>
-      <c r="P180">
-        <v>0</v>
-      </c>
-      <c r="Q180">
-        <v>0</v>
-      </c>
-      <c r="R180">
-        <v>0</v>
-      </c>
-      <c r="S180">
-        <v>0</v>
-      </c>
-      <c r="T180">
-        <v>0</v>
-      </c>
-      <c r="U180">
-        <v>0</v>
-      </c>
-      <c r="V180">
-        <v>0</v>
-      </c>
-      <c r="W180">
-        <v>362054.1554679333</v>
-      </c>
-      <c r="X180">
-        <v>15</v>
-      </c>
-      <c r="Y180">
-        <v>15</v>
-      </c>
-      <c r="Z180">
-        <v>15</v>
-      </c>
-      <c r="AA180">
-        <v>15</v>
-      </c>
-      <c r="AB180">
-        <v>0</v>
-      </c>
-      <c r="AC180">
-        <v>0</v>
-      </c>
-      <c r="AD180">
-        <v>0</v>
-      </c>
-      <c r="AE180">
-        <v>1498181.4168192</v>
-      </c>
-      <c r="AF180">
-        <v>1.001213860458009E-05</v>
-      </c>
-      <c r="AG180">
-        <v>0</v>
-      </c>
-      <c r="AH180">
-        <v>0</v>
-      </c>
-      <c r="AJ180">
-        <v>0</v>
-      </c>
-      <c r="AK180">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="181" spans="1:37">
-      <c r="A181" s="2">
-        <v>44089</v>
-      </c>
-      <c r="B181">
-        <v>179</v>
-      </c>
-      <c r="C181">
-        <v>1137715.655858824</v>
-      </c>
-      <c r="D181">
-        <v>1138198.442082663</v>
-      </c>
-      <c r="E181">
-        <v>0</v>
-      </c>
-      <c r="F181">
-        <v>0</v>
-      </c>
-      <c r="G181">
-        <v>1136112.261351267</v>
-      </c>
-      <c r="H181">
-        <v>690685.0257366077</v>
-      </c>
-      <c r="I181">
-        <v>24252.2503426687</v>
-      </c>
-      <c r="J181">
-        <v>5105.730586805043</v>
-      </c>
-      <c r="K181">
-        <v>1818.5831808</v>
-      </c>
-      <c r="L181">
-        <v>0</v>
-      </c>
-      <c r="M181">
-        <v>0</v>
-      </c>
-      <c r="N181">
-        <v>0</v>
-      </c>
-      <c r="O181">
-        <v>0</v>
-      </c>
-      <c r="P181">
-        <v>0</v>
-      </c>
-      <c r="Q181">
-        <v>0</v>
-      </c>
-      <c r="R181">
-        <v>0</v>
-      </c>
-      <c r="S181">
-        <v>0</v>
-      </c>
-      <c r="T181">
-        <v>0</v>
-      </c>
-      <c r="U181">
-        <v>0</v>
-      </c>
-      <c r="V181">
-        <v>0</v>
-      </c>
-      <c r="W181">
-        <v>362054.1554679333</v>
-      </c>
-      <c r="X181">
-        <v>15</v>
-      </c>
-      <c r="Y181">
-        <v>15</v>
-      </c>
-      <c r="Z181">
-        <v>15</v>
-      </c>
-      <c r="AA181">
-        <v>15</v>
-      </c>
-      <c r="AB181">
-        <v>0</v>
-      </c>
-      <c r="AC181">
-        <v>0</v>
-      </c>
-      <c r="AD181">
-        <v>0</v>
-      </c>
-      <c r="AE181">
-        <v>1498181.4168192</v>
-      </c>
-      <c r="AF181">
-        <v>1.001213860458009E-05</v>
-      </c>
-      <c r="AG181">
-        <v>0</v>
-      </c>
-      <c r="AH181">
-        <v>0</v>
-      </c>
-      <c r="AJ181">
-        <v>0</v>
-      </c>
-      <c r="AK181">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="182" spans="1:37">
-      <c r="A182" s="2">
-        <v>44090</v>
-      </c>
-      <c r="B182">
-        <v>180</v>
-      </c>
-      <c r="C182">
-        <v>1137715.655858824</v>
-      </c>
-      <c r="D182">
-        <v>1138198.442082663</v>
-      </c>
-      <c r="E182">
-        <v>0</v>
-      </c>
-      <c r="F182">
-        <v>0</v>
-      </c>
-      <c r="G182">
-        <v>1136112.261351267</v>
-      </c>
-      <c r="H182">
-        <v>690685.0257366077</v>
-      </c>
-      <c r="I182">
-        <v>24252.2503426687</v>
-      </c>
-      <c r="J182">
-        <v>5105.730586805043</v>
-      </c>
-      <c r="K182">
-        <v>1818.5831808</v>
-      </c>
-      <c r="L182">
-        <v>0</v>
-      </c>
-      <c r="M182">
-        <v>0</v>
-      </c>
-      <c r="N182">
-        <v>0</v>
-      </c>
-      <c r="O182">
-        <v>0</v>
-      </c>
-      <c r="P182">
-        <v>0</v>
-      </c>
-      <c r="Q182">
-        <v>0</v>
-      </c>
-      <c r="R182">
-        <v>0</v>
-      </c>
-      <c r="S182">
-        <v>0</v>
-      </c>
-      <c r="T182">
-        <v>0</v>
-      </c>
-      <c r="U182">
-        <v>0</v>
-      </c>
-      <c r="V182">
-        <v>0</v>
-      </c>
-      <c r="W182">
-        <v>362054.1554679333</v>
-      </c>
-      <c r="X182">
-        <v>15</v>
-      </c>
-      <c r="Y182">
-        <v>15</v>
-      </c>
-      <c r="Z182">
-        <v>15</v>
-      </c>
-      <c r="AA182">
-        <v>15</v>
-      </c>
-      <c r="AB182">
-        <v>0</v>
-      </c>
-      <c r="AC182">
-        <v>0</v>
-      </c>
-      <c r="AD182">
-        <v>0</v>
-      </c>
-      <c r="AE182">
-        <v>1498181.4168192</v>
-      </c>
-      <c r="AF182">
-        <v>1.001213860458009E-05</v>
-      </c>
-      <c r="AG182">
-        <v>0</v>
-      </c>
-      <c r="AH182">
-        <v>0</v>
-      </c>
-      <c r="AJ182">
-        <v>0</v>
-      </c>
-      <c r="AK182">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="183" spans="1:37">
-      <c r="A183" s="2">
-        <v>44091</v>
-      </c>
-      <c r="B183">
-        <v>181</v>
-      </c>
-      <c r="C183">
-        <v>1137715.655858824</v>
-      </c>
-      <c r="D183">
-        <v>1138198.442082663</v>
-      </c>
-      <c r="E183">
-        <v>0</v>
-      </c>
-      <c r="F183">
-        <v>0</v>
-      </c>
-      <c r="G183">
-        <v>1136127.261351267</v>
-      </c>
-      <c r="H183">
-        <v>690685.0257366077</v>
-      </c>
-      <c r="I183">
-        <v>24252.2503426687</v>
-      </c>
-      <c r="J183">
-        <v>5105.730586805043</v>
-      </c>
-      <c r="K183">
-        <v>1818.5831808</v>
-      </c>
-      <c r="L183">
-        <v>0</v>
-      </c>
-      <c r="M183">
-        <v>0</v>
-      </c>
-      <c r="N183">
-        <v>0</v>
-      </c>
-      <c r="O183">
-        <v>0</v>
-      </c>
-      <c r="P183">
-        <v>0</v>
-      </c>
-      <c r="Q183">
-        <v>15</v>
-      </c>
-      <c r="R183">
-        <v>0</v>
-      </c>
-      <c r="S183">
-        <v>0</v>
-      </c>
-      <c r="T183">
-        <v>0</v>
-      </c>
-      <c r="U183">
-        <v>0</v>
-      </c>
-      <c r="V183">
-        <v>0</v>
-      </c>
-      <c r="W183">
-        <v>362054.1554679333</v>
-      </c>
-      <c r="X183">
-        <v>0</v>
-      </c>
-      <c r="Y183">
-        <v>0</v>
-      </c>
-      <c r="Z183">
-        <v>0</v>
-      </c>
-      <c r="AA183">
-        <v>0</v>
-      </c>
-      <c r="AB183">
-        <v>0</v>
-      </c>
-      <c r="AC183">
-        <v>0</v>
-      </c>
-      <c r="AD183">
-        <v>0</v>
-      </c>
-      <c r="AE183">
-        <v>1498181.4168192</v>
-      </c>
-      <c r="AF183">
-        <v>0</v>
-      </c>
-      <c r="AG183">
-        <v>0</v>
-      </c>
-      <c r="AH183">
-        <v>0</v>
-      </c>
-      <c r="AJ183">
-        <v>0</v>
-      </c>
-      <c r="AK183">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="184" spans="1:37">
-      <c r="A184" s="2">
-        <v>44092</v>
-      </c>
-      <c r="B184">
-        <v>182</v>
-      </c>
-      <c r="C184">
-        <v>1137715.655858824</v>
-      </c>
-      <c r="D184">
-        <v>1138198.442082663</v>
-      </c>
-      <c r="E184">
-        <v>0</v>
-      </c>
-      <c r="F184">
-        <v>0</v>
-      </c>
-      <c r="G184">
-        <v>1136127.261351267</v>
-      </c>
-      <c r="H184">
-        <v>690685.0257366077</v>
-      </c>
-      <c r="I184">
-        <v>24252.2503426687</v>
-      </c>
-      <c r="J184">
-        <v>5105.730586805043</v>
-      </c>
-      <c r="K184">
-        <v>1818.5831808</v>
-      </c>
-      <c r="L184">
-        <v>0</v>
-      </c>
-      <c r="M184">
-        <v>0</v>
-      </c>
-      <c r="N184">
-        <v>0</v>
-      </c>
-      <c r="O184">
-        <v>0</v>
-      </c>
-      <c r="P184">
-        <v>0</v>
-      </c>
-      <c r="Q184">
-        <v>0</v>
-      </c>
-      <c r="R184">
-        <v>0</v>
-      </c>
-      <c r="S184">
-        <v>0</v>
-      </c>
-      <c r="T184">
-        <v>0</v>
-      </c>
-      <c r="U184">
-        <v>0</v>
-      </c>
-      <c r="V184">
-        <v>0</v>
-      </c>
-      <c r="W184">
-        <v>362054.1554679333</v>
-      </c>
-      <c r="X184">
-        <v>0</v>
-      </c>
-      <c r="Y184">
-        <v>0</v>
-      </c>
-      <c r="Z184">
-        <v>0</v>
-      </c>
-      <c r="AA184">
-        <v>0</v>
-      </c>
-      <c r="AB184">
-        <v>0</v>
-      </c>
-      <c r="AC184">
-        <v>0</v>
-      </c>
-      <c r="AD184">
-        <v>0</v>
-      </c>
-      <c r="AE184">
-        <v>1498181.4168192</v>
-      </c>
-      <c r="AF184">
-        <v>0</v>
-      </c>
-      <c r="AG184">
-        <v>0</v>
-      </c>
-      <c r="AH184">
-        <v>0</v>
-      </c>
-      <c r="AJ184">
-        <v>0</v>
-      </c>
-      <c r="AK184">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="185" spans="1:37">
-      <c r="A185" s="2">
-        <v>44093</v>
-      </c>
-      <c r="B185">
-        <v>183</v>
-      </c>
-      <c r="C185">
-        <v>1137715.655858824</v>
-      </c>
-      <c r="D185">
-        <v>1138198.442082663</v>
-      </c>
-      <c r="E185">
-        <v>0</v>
-      </c>
-      <c r="F185">
-        <v>0</v>
-      </c>
-      <c r="G185">
-        <v>1136127.261351267</v>
-      </c>
-      <c r="H185">
-        <v>690685.0257366077</v>
-      </c>
-      <c r="I185">
-        <v>24252.2503426687</v>
-      </c>
-      <c r="J185">
-        <v>5105.730586805043</v>
-      </c>
-      <c r="K185">
-        <v>1818.5831808</v>
-      </c>
-      <c r="L185">
-        <v>0</v>
-      </c>
-      <c r="M185">
-        <v>0</v>
-      </c>
-      <c r="N185">
-        <v>0</v>
-      </c>
-      <c r="O185">
-        <v>0</v>
-      </c>
-      <c r="P185">
-        <v>0</v>
-      </c>
-      <c r="Q185">
-        <v>0</v>
-      </c>
-      <c r="R185">
-        <v>0</v>
-      </c>
-      <c r="S185">
-        <v>0</v>
-      </c>
-      <c r="T185">
-        <v>0</v>
-      </c>
-      <c r="U185">
-        <v>0</v>
-      </c>
-      <c r="V185">
-        <v>0</v>
-      </c>
-      <c r="W185">
-        <v>362054.1554679333</v>
-      </c>
-      <c r="X185">
-        <v>0</v>
-      </c>
-      <c r="Y185">
-        <v>0</v>
-      </c>
-      <c r="Z185">
-        <v>0</v>
-      </c>
-      <c r="AA185">
-        <v>0</v>
-      </c>
-      <c r="AB185">
-        <v>0</v>
-      </c>
-      <c r="AC185">
-        <v>0</v>
-      </c>
-      <c r="AD185">
-        <v>0</v>
-      </c>
-      <c r="AE185">
-        <v>1498181.4168192</v>
-      </c>
-      <c r="AF185">
-        <v>0</v>
-      </c>
-      <c r="AG185">
-        <v>0</v>
-      </c>
-      <c r="AH185">
-        <v>0</v>
-      </c>
-      <c r="AJ185">
-        <v>0</v>
-      </c>
-      <c r="AK185">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="186" spans="1:37">
-      <c r="A186" s="2">
-        <v>44094</v>
-      </c>
-      <c r="B186">
-        <v>184</v>
-      </c>
-      <c r="C186">
-        <v>1137715.655858824</v>
-      </c>
-      <c r="D186">
-        <v>1138198.442082663</v>
-      </c>
-      <c r="E186">
-        <v>0</v>
-      </c>
-      <c r="F186">
-        <v>0</v>
-      </c>
-      <c r="G186">
-        <v>1136127.261351267</v>
-      </c>
-      <c r="H186">
-        <v>690685.0257366077</v>
-      </c>
-      <c r="I186">
-        <v>24252.2503426687</v>
-      </c>
-      <c r="J186">
-        <v>5105.730586805043</v>
-      </c>
-      <c r="K186">
-        <v>1818.5831808</v>
-      </c>
-      <c r="L186">
-        <v>0</v>
-      </c>
-      <c r="M186">
-        <v>0</v>
-      </c>
-      <c r="N186">
-        <v>0</v>
-      </c>
-      <c r="O186">
-        <v>0</v>
-      </c>
-      <c r="P186">
-        <v>0</v>
-      </c>
-      <c r="Q186">
-        <v>0</v>
-      </c>
-      <c r="R186">
-        <v>0</v>
-      </c>
-      <c r="S186">
-        <v>0</v>
-      </c>
-      <c r="T186">
-        <v>0</v>
-      </c>
-      <c r="U186">
-        <v>0</v>
-      </c>
-      <c r="V186">
-        <v>0</v>
-      </c>
-      <c r="W186">
-        <v>362054.1554679333</v>
-      </c>
-      <c r="X186">
-        <v>0</v>
-      </c>
-      <c r="Y186">
-        <v>0</v>
-      </c>
-      <c r="Z186">
-        <v>0</v>
-      </c>
-      <c r="AA186">
-        <v>0</v>
-      </c>
-      <c r="AB186">
-        <v>0</v>
-      </c>
-      <c r="AC186">
-        <v>0</v>
-      </c>
-      <c r="AD186">
-        <v>0</v>
-      </c>
-      <c r="AE186">
-        <v>1498181.4168192</v>
-      </c>
-      <c r="AF186">
-        <v>0</v>
-      </c>
-      <c r="AG186">
-        <v>0</v>
-      </c>
-      <c r="AH186">
-        <v>0</v>
-      </c>
-      <c r="AJ186">
-        <v>0</v>
-      </c>
-      <c r="AK186">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="187" spans="1:37">
-      <c r="A187" s="2">
-        <v>44095</v>
-      </c>
-      <c r="B187">
-        <v>185</v>
-      </c>
-      <c r="C187">
-        <v>1137715.655858824</v>
-      </c>
-      <c r="D187">
-        <v>1138198.442082663</v>
-      </c>
-      <c r="E187">
-        <v>0</v>
-      </c>
-      <c r="F187">
-        <v>0</v>
-      </c>
-      <c r="G187">
-        <v>1136127.261351267</v>
-      </c>
-      <c r="H187">
-        <v>690685.0257366077</v>
-      </c>
-      <c r="I187">
-        <v>24252.2503426687</v>
-      </c>
-      <c r="J187">
-        <v>5105.730586805043</v>
-      </c>
-      <c r="K187">
-        <v>1818.5831808</v>
-      </c>
-      <c r="L187">
-        <v>0</v>
-      </c>
-      <c r="M187">
-        <v>0</v>
-      </c>
-      <c r="N187">
-        <v>0</v>
-      </c>
-      <c r="O187">
-        <v>0</v>
-      </c>
-      <c r="P187">
-        <v>0</v>
-      </c>
-      <c r="Q187">
-        <v>0</v>
-      </c>
-      <c r="R187">
-        <v>0</v>
-      </c>
-      <c r="S187">
-        <v>0</v>
-      </c>
-      <c r="T187">
-        <v>0</v>
-      </c>
-      <c r="U187">
-        <v>0</v>
-      </c>
-      <c r="V187">
-        <v>0</v>
-      </c>
-      <c r="W187">
-        <v>362054.1554679333</v>
-      </c>
-      <c r="X187">
-        <v>0</v>
-      </c>
-      <c r="Y187">
-        <v>0</v>
-      </c>
-      <c r="Z187">
-        <v>0</v>
-      </c>
-      <c r="AA187">
-        <v>0</v>
-      </c>
-      <c r="AB187">
-        <v>0</v>
-      </c>
-      <c r="AC187">
-        <v>0</v>
-      </c>
-      <c r="AD187">
-        <v>0</v>
-      </c>
-      <c r="AE187">
-        <v>1498181.4168192</v>
-      </c>
-      <c r="AF187">
-        <v>0</v>
-      </c>
-      <c r="AG187">
-        <v>0</v>
-      </c>
-      <c r="AH187">
-        <v>0</v>
-      </c>
-      <c r="AJ187">
-        <v>0</v>
-      </c>
-      <c r="AK187">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="188" spans="1:37">
-      <c r="A188" s="2">
-        <v>44096</v>
-      </c>
-      <c r="B188">
-        <v>186</v>
-      </c>
-      <c r="C188">
-        <v>1137715.655858824</v>
-      </c>
-      <c r="D188">
-        <v>1138198.442082663</v>
-      </c>
-      <c r="E188">
-        <v>0</v>
-      </c>
-      <c r="F188">
-        <v>0</v>
-      </c>
-      <c r="G188">
-        <v>1136127.261351267</v>
-      </c>
-      <c r="H188">
-        <v>690685.0257366077</v>
-      </c>
-      <c r="I188">
-        <v>24252.2503426687</v>
-      </c>
-      <c r="J188">
-        <v>5105.730586805043</v>
-      </c>
-      <c r="K188">
-        <v>1818.5831808</v>
-      </c>
-      <c r="L188">
-        <v>0</v>
-      </c>
-      <c r="M188">
-        <v>0</v>
-      </c>
-      <c r="N188">
-        <v>0</v>
-      </c>
-      <c r="O188">
-        <v>0</v>
-      </c>
-      <c r="P188">
-        <v>0</v>
-      </c>
-      <c r="Q188">
-        <v>0</v>
-      </c>
-      <c r="R188">
-        <v>0</v>
-      </c>
-      <c r="S188">
-        <v>0</v>
-      </c>
-      <c r="T188">
-        <v>0</v>
-      </c>
-      <c r="U188">
-        <v>0</v>
-      </c>
-      <c r="V188">
-        <v>0</v>
-      </c>
-      <c r="W188">
-        <v>362054.1554679333</v>
-      </c>
-      <c r="X188">
-        <v>0</v>
-      </c>
-      <c r="Y188">
-        <v>0</v>
-      </c>
-      <c r="Z188">
-        <v>0</v>
-      </c>
-      <c r="AA188">
-        <v>0</v>
-      </c>
-      <c r="AB188">
-        <v>0</v>
-      </c>
-      <c r="AC188">
-        <v>0</v>
-      </c>
-      <c r="AD188">
-        <v>0</v>
-      </c>
-      <c r="AE188">
-        <v>1498181.4168192</v>
-      </c>
-      <c r="AF188">
-        <v>0</v>
-      </c>
-      <c r="AG188">
-        <v>0</v>
-      </c>
-      <c r="AH188">
-        <v>0</v>
-      </c>
-      <c r="AJ188">
-        <v>0</v>
-      </c>
-      <c r="AK188">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="189" spans="1:37">
-      <c r="A189" s="2">
-        <v>44097</v>
-      </c>
-      <c r="B189">
-        <v>187</v>
-      </c>
-      <c r="C189">
-        <v>1137715.655858824</v>
-      </c>
-      <c r="D189">
-        <v>1138198.442082663</v>
-      </c>
-      <c r="E189">
-        <v>0</v>
-      </c>
-      <c r="F189">
-        <v>0</v>
-      </c>
-      <c r="G189">
-        <v>1136127.261351267</v>
-      </c>
-      <c r="H189">
-        <v>690685.0257366077</v>
-      </c>
-      <c r="I189">
-        <v>24252.2503426687</v>
-      </c>
-      <c r="J189">
-        <v>5105.730586805043</v>
-      </c>
-      <c r="K189">
-        <v>1818.5831808</v>
-      </c>
-      <c r="L189">
-        <v>0</v>
-      </c>
-      <c r="M189">
-        <v>0</v>
-      </c>
-      <c r="N189">
-        <v>0</v>
-      </c>
-      <c r="O189">
-        <v>0</v>
-      </c>
-      <c r="P189">
-        <v>0</v>
-      </c>
-      <c r="Q189">
-        <v>0</v>
-      </c>
-      <c r="R189">
-        <v>0</v>
-      </c>
-      <c r="S189">
-        <v>0</v>
-      </c>
-      <c r="T189">
-        <v>0</v>
-      </c>
-      <c r="U189">
-        <v>0</v>
-      </c>
-      <c r="V189">
-        <v>0</v>
-      </c>
-      <c r="W189">
-        <v>362054.1554679333</v>
-      </c>
-      <c r="X189">
-        <v>0</v>
-      </c>
-      <c r="Y189">
-        <v>0</v>
-      </c>
-      <c r="Z189">
-        <v>0</v>
-      </c>
-      <c r="AA189">
-        <v>0</v>
-      </c>
-      <c r="AB189">
-        <v>0</v>
-      </c>
-      <c r="AC189">
-        <v>0</v>
-      </c>
-      <c r="AD189">
-        <v>0</v>
-      </c>
-      <c r="AE189">
-        <v>1498181.4168192</v>
-      </c>
-      <c r="AF189">
-        <v>0</v>
-      </c>
-      <c r="AG189">
-        <v>0</v>
-      </c>
-      <c r="AH189">
-        <v>0</v>
-      </c>
-      <c r="AJ189">
-        <v>0</v>
-      </c>
-      <c r="AK189">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="190" spans="1:37">
-      <c r="A190" s="2">
-        <v>44098</v>
-      </c>
-      <c r="B190">
-        <v>188</v>
-      </c>
-      <c r="C190">
-        <v>1137715.655858824</v>
-      </c>
-      <c r="D190">
-        <v>1138198.442082663</v>
-      </c>
-      <c r="E190">
-        <v>0</v>
-      </c>
-      <c r="F190">
-        <v>0</v>
-      </c>
-      <c r="G190">
-        <v>1136127.261351267</v>
-      </c>
-      <c r="H190">
-        <v>690685.0257366077</v>
-      </c>
-      <c r="I190">
-        <v>24252.2503426687</v>
-      </c>
-      <c r="J190">
-        <v>5105.730586805043</v>
-      </c>
-      <c r="K190">
-        <v>1818.5831808</v>
-      </c>
-      <c r="L190">
-        <v>0</v>
-      </c>
-      <c r="M190">
-        <v>0</v>
-      </c>
-      <c r="N190">
-        <v>0</v>
-      </c>
-      <c r="O190">
-        <v>0</v>
-      </c>
-      <c r="P190">
-        <v>0</v>
-      </c>
-      <c r="Q190">
-        <v>0</v>
-      </c>
-      <c r="R190">
-        <v>0</v>
-      </c>
-      <c r="S190">
-        <v>0</v>
-      </c>
-      <c r="T190">
-        <v>0</v>
-      </c>
-      <c r="U190">
-        <v>0</v>
-      </c>
-      <c r="V190">
-        <v>0</v>
-      </c>
-      <c r="W190">
-        <v>362054.1554679333</v>
-      </c>
-      <c r="X190">
-        <v>0</v>
-      </c>
-      <c r="Y190">
-        <v>0</v>
-      </c>
-      <c r="Z190">
-        <v>0</v>
-      </c>
-      <c r="AA190">
-        <v>0</v>
-      </c>
-      <c r="AB190">
-        <v>0</v>
-      </c>
-      <c r="AC190">
-        <v>0</v>
-      </c>
-      <c r="AD190">
-        <v>0</v>
-      </c>
-      <c r="AE190">
-        <v>1498181.4168192</v>
-      </c>
-      <c r="AF190">
-        <v>0</v>
-      </c>
-      <c r="AG190">
-        <v>0</v>
-      </c>
-      <c r="AH190">
-        <v>0</v>
-      </c>
-      <c r="AJ190">
-        <v>0</v>
-      </c>
-      <c r="AK190">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="191" spans="1:37">
-      <c r="A191" s="2">
-        <v>44099</v>
-      </c>
-      <c r="B191">
-        <v>189</v>
-      </c>
-      <c r="C191">
-        <v>1137715.655858824</v>
-      </c>
-      <c r="D191">
-        <v>1138198.442082663</v>
-      </c>
-      <c r="E191">
-        <v>0</v>
-      </c>
-      <c r="F191">
-        <v>0</v>
-      </c>
-      <c r="G191">
-        <v>1136127.261351267</v>
-      </c>
-      <c r="H191">
-        <v>690685.0257366077</v>
-      </c>
-      <c r="I191">
-        <v>24252.2503426687</v>
-      </c>
-      <c r="J191">
-        <v>5105.730586805043</v>
-      </c>
-      <c r="K191">
-        <v>1818.5831808</v>
-      </c>
-      <c r="L191">
-        <v>0</v>
-      </c>
-      <c r="M191">
-        <v>0</v>
-      </c>
-      <c r="N191">
-        <v>0</v>
-      </c>
-      <c r="O191">
-        <v>0</v>
-      </c>
-      <c r="P191">
-        <v>0</v>
-      </c>
-      <c r="Q191">
-        <v>0</v>
-      </c>
-      <c r="R191">
-        <v>0</v>
-      </c>
-      <c r="S191">
-        <v>0</v>
-      </c>
-      <c r="T191">
-        <v>0</v>
-      </c>
-      <c r="U191">
-        <v>0</v>
-      </c>
-      <c r="V191">
-        <v>0</v>
-      </c>
-      <c r="W191">
-        <v>362054.1554679333</v>
-      </c>
-      <c r="X191">
-        <v>0</v>
-      </c>
-      <c r="Y191">
-        <v>0</v>
-      </c>
-      <c r="Z191">
-        <v>0</v>
-      </c>
-      <c r="AA191">
-        <v>0</v>
-      </c>
-      <c r="AB191">
-        <v>0</v>
-      </c>
-      <c r="AC191">
-        <v>0</v>
-      </c>
-      <c r="AD191">
-        <v>0</v>
-      </c>
-      <c r="AE191">
-        <v>1498181.4168192</v>
-      </c>
-      <c r="AF191">
-        <v>0</v>
-      </c>
-      <c r="AG191">
-        <v>0</v>
-      </c>
-      <c r="AH191">
-        <v>0</v>
-      </c>
-      <c r="AJ191">
-        <v>0</v>
-      </c>
-      <c r="AK191">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="192" spans="1:37">
-      <c r="A192" s="2">
-        <v>44100</v>
-      </c>
-      <c r="B192">
-        <v>190</v>
-      </c>
-      <c r="C192">
-        <v>1137715.655858824</v>
-      </c>
-      <c r="D192">
-        <v>1138198.442082663</v>
-      </c>
-      <c r="E192">
-        <v>0</v>
-      </c>
-      <c r="F192">
-        <v>0</v>
-      </c>
-      <c r="G192">
-        <v>1136127.261351267</v>
-      </c>
-      <c r="H192">
-        <v>690685.0257366077</v>
-      </c>
-      <c r="I192">
-        <v>24252.2503426687</v>
-      </c>
-      <c r="J192">
-        <v>5105.730586805043</v>
-      </c>
-      <c r="K192">
-        <v>1818.5831808</v>
-      </c>
-      <c r="L192">
-        <v>0</v>
-      </c>
-      <c r="M192">
-        <v>0</v>
-      </c>
-      <c r="N192">
-        <v>0</v>
-      </c>
-      <c r="O192">
-        <v>0</v>
-      </c>
-      <c r="P192">
-        <v>0</v>
-      </c>
-      <c r="Q192">
-        <v>0</v>
-      </c>
-      <c r="R192">
-        <v>0</v>
-      </c>
-      <c r="S192">
-        <v>0</v>
-      </c>
-      <c r="T192">
-        <v>0</v>
-      </c>
-      <c r="U192">
-        <v>0</v>
-      </c>
-      <c r="V192">
-        <v>0</v>
-      </c>
-      <c r="W192">
-        <v>362054.1554679333</v>
-      </c>
-      <c r="X192">
-        <v>0</v>
-      </c>
-      <c r="Y192">
-        <v>0</v>
-      </c>
-      <c r="Z192">
-        <v>0</v>
-      </c>
-      <c r="AA192">
-        <v>0</v>
-      </c>
-      <c r="AB192">
-        <v>0</v>
-      </c>
-      <c r="AC192">
-        <v>0</v>
-      </c>
-      <c r="AD192">
-        <v>0</v>
-      </c>
-      <c r="AE192">
-        <v>1498181.4168192</v>
-      </c>
-      <c r="AF192">
-        <v>0</v>
-      </c>
-      <c r="AG192">
-        <v>0</v>
-      </c>
-      <c r="AH192">
-        <v>0</v>
-      </c>
-      <c r="AJ192">
-        <v>0</v>
-      </c>
-      <c r="AK192">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="193" spans="1:37">
-      <c r="A193" s="2">
-        <v>44101</v>
-      </c>
-      <c r="B193">
-        <v>191</v>
-      </c>
-      <c r="C193">
-        <v>1137715.655858824</v>
-      </c>
-      <c r="D193">
-        <v>1138198.442082663</v>
-      </c>
-      <c r="E193">
-        <v>0</v>
-      </c>
-      <c r="F193">
-        <v>0</v>
-      </c>
-      <c r="G193">
-        <v>1136127.261351267</v>
-      </c>
-      <c r="H193">
-        <v>690685.0257366077</v>
-      </c>
-      <c r="I193">
-        <v>24252.2503426687</v>
-      </c>
-      <c r="J193">
-        <v>5105.730586805043</v>
-      </c>
-      <c r="K193">
-        <v>1818.5831808</v>
-      </c>
-      <c r="L193">
-        <v>0</v>
-      </c>
-      <c r="M193">
-        <v>0</v>
-      </c>
-      <c r="N193">
-        <v>0</v>
-      </c>
-      <c r="O193">
-        <v>0</v>
-      </c>
-      <c r="P193">
-        <v>0</v>
-      </c>
-      <c r="Q193">
-        <v>0</v>
-      </c>
-      <c r="R193">
-        <v>0</v>
-      </c>
-      <c r="S193">
-        <v>0</v>
-      </c>
-      <c r="T193">
-        <v>0</v>
-      </c>
-      <c r="U193">
-        <v>0</v>
-      </c>
-      <c r="V193">
-        <v>0</v>
-      </c>
-      <c r="W193">
-        <v>362054.1554679333</v>
-      </c>
-      <c r="X193">
-        <v>0</v>
-      </c>
-      <c r="Y193">
-        <v>0</v>
-      </c>
-      <c r="Z193">
-        <v>0</v>
-      </c>
-      <c r="AA193">
-        <v>0</v>
-      </c>
-      <c r="AB193">
-        <v>0</v>
-      </c>
-      <c r="AC193">
-        <v>0</v>
-      </c>
-      <c r="AD193">
-        <v>0</v>
-      </c>
-      <c r="AE193">
-        <v>1498181.4168192</v>
-      </c>
-      <c r="AF193">
-        <v>0</v>
-      </c>
-      <c r="AG193">
-        <v>0</v>
-      </c>
-      <c r="AH193">
-        <v>0</v>
-      </c>
-      <c r="AJ193">
-        <v>0</v>
-      </c>
-      <c r="AK193">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="194" spans="1:37">
-      <c r="A194" s="2">
-        <v>44102</v>
-      </c>
-      <c r="B194">
-        <v>192</v>
-      </c>
-      <c r="C194">
-        <v>1137715.655858824</v>
-      </c>
-      <c r="D194">
-        <v>1138198.442082663</v>
-      </c>
-      <c r="E194">
-        <v>0</v>
-      </c>
-      <c r="F194">
-        <v>0</v>
-      </c>
-      <c r="G194">
-        <v>1136127.261351267</v>
-      </c>
-      <c r="H194">
-        <v>690685.0257366077</v>
-      </c>
-      <c r="I194">
-        <v>24252.2503426687</v>
-      </c>
-      <c r="J194">
-        <v>5105.730586805043</v>
-      </c>
-      <c r="K194">
-        <v>1818.5831808</v>
-      </c>
-      <c r="L194">
-        <v>0</v>
-      </c>
-      <c r="M194">
-        <v>0</v>
-      </c>
-      <c r="N194">
-        <v>0</v>
-      </c>
-      <c r="O194">
-        <v>0</v>
-      </c>
-      <c r="P194">
-        <v>0</v>
-      </c>
-      <c r="Q194">
-        <v>0</v>
-      </c>
-      <c r="R194">
-        <v>0</v>
-      </c>
-      <c r="S194">
-        <v>0</v>
-      </c>
-      <c r="T194">
-        <v>0</v>
-      </c>
-      <c r="U194">
-        <v>0</v>
-      </c>
-      <c r="V194">
-        <v>0</v>
-      </c>
-      <c r="W194">
-        <v>362054.1554679333</v>
-      </c>
-      <c r="X194">
-        <v>0</v>
-      </c>
-      <c r="Y194">
-        <v>0</v>
-      </c>
-      <c r="Z194">
-        <v>0</v>
-      </c>
-      <c r="AA194">
-        <v>0</v>
-      </c>
-      <c r="AB194">
-        <v>0</v>
-      </c>
-      <c r="AC194">
-        <v>0</v>
-      </c>
-      <c r="AD194">
-        <v>0</v>
-      </c>
-      <c r="AE194">
-        <v>1498181.4168192</v>
-      </c>
-      <c r="AF194">
-        <v>0</v>
-      </c>
-      <c r="AG194">
-        <v>0</v>
-      </c>
-      <c r="AH194">
-        <v>0</v>
-      </c>
-      <c r="AJ194">
-        <v>0</v>
-      </c>
-      <c r="AK194">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="195" spans="1:37">
-      <c r="A195" s="2">
-        <v>44103</v>
-      </c>
-      <c r="B195">
-        <v>193</v>
-      </c>
-      <c r="C195">
-        <v>1137715.655858824</v>
-      </c>
-      <c r="D195">
-        <v>1138198.442082663</v>
-      </c>
-      <c r="E195">
-        <v>0</v>
-      </c>
-      <c r="F195">
-        <v>0</v>
-      </c>
-      <c r="G195">
-        <v>1136127.261351267</v>
-      </c>
-      <c r="H195">
-        <v>690685.0257366077</v>
-      </c>
-      <c r="I195">
-        <v>24252.2503426687</v>
-      </c>
-      <c r="J195">
-        <v>5105.730586805043</v>
-      </c>
-      <c r="K195">
-        <v>1818.5831808</v>
-      </c>
-      <c r="L195">
-        <v>0</v>
-      </c>
-      <c r="M195">
-        <v>0</v>
-      </c>
-      <c r="N195">
-        <v>0</v>
-      </c>
-      <c r="O195">
-        <v>0</v>
-      </c>
-      <c r="P195">
-        <v>0</v>
-      </c>
-      <c r="Q195">
-        <v>0</v>
-      </c>
-      <c r="R195">
-        <v>0</v>
-      </c>
-      <c r="S195">
-        <v>0</v>
-      </c>
-      <c r="T195">
-        <v>0</v>
-      </c>
-      <c r="U195">
-        <v>0</v>
-      </c>
-      <c r="V195">
-        <v>0</v>
-      </c>
-      <c r="W195">
-        <v>362054.1554679333</v>
-      </c>
-      <c r="X195">
-        <v>0</v>
-      </c>
-      <c r="Y195">
-        <v>0</v>
-      </c>
-      <c r="Z195">
-        <v>0</v>
-      </c>
-      <c r="AA195">
-        <v>0</v>
-      </c>
-      <c r="AB195">
-        <v>0</v>
-      </c>
-      <c r="AC195">
-        <v>0</v>
-      </c>
-      <c r="AD195">
-        <v>0</v>
-      </c>
-      <c r="AE195">
-        <v>1498181.4168192</v>
-      </c>
-      <c r="AF195">
-        <v>0</v>
-      </c>
-      <c r="AG195">
-        <v>0</v>
-      </c>
-      <c r="AH195">
-        <v>0</v>
-      </c>
-      <c r="AJ195">
-        <v>0</v>
-      </c>
-      <c r="AK195">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="196" spans="1:37">
-      <c r="A196" s="2">
-        <v>44104</v>
-      </c>
-      <c r="B196">
-        <v>194</v>
-      </c>
-      <c r="C196">
-        <v>1137715.655858824</v>
-      </c>
-      <c r="D196">
-        <v>1138198.442082663</v>
-      </c>
-      <c r="E196">
-        <v>0</v>
-      </c>
-      <c r="F196">
-        <v>0</v>
-      </c>
-      <c r="G196">
-        <v>1136127.261351267</v>
-      </c>
-      <c r="H196">
-        <v>690685.0257366077</v>
-      </c>
-      <c r="I196">
-        <v>24252.2503426687</v>
-      </c>
-      <c r="J196">
-        <v>5105.730586805043</v>
-      </c>
-      <c r="K196">
-        <v>1818.5831808</v>
-      </c>
-      <c r="L196">
-        <v>0</v>
-      </c>
-      <c r="M196">
-        <v>0</v>
-      </c>
-      <c r="N196">
-        <v>0</v>
-      </c>
-      <c r="O196">
-        <v>0</v>
-      </c>
-      <c r="P196">
-        <v>0</v>
-      </c>
-      <c r="Q196">
-        <v>0</v>
-      </c>
-      <c r="R196">
-        <v>0</v>
-      </c>
-      <c r="S196">
-        <v>0</v>
-      </c>
-      <c r="T196">
-        <v>0</v>
-      </c>
-      <c r="U196">
-        <v>0</v>
-      </c>
-      <c r="V196">
-        <v>0</v>
-      </c>
-      <c r="W196">
-        <v>362054.1554679333</v>
-      </c>
-      <c r="X196">
-        <v>0</v>
-      </c>
-      <c r="Y196">
-        <v>0</v>
-      </c>
-      <c r="Z196">
-        <v>0</v>
-      </c>
-      <c r="AA196">
-        <v>0</v>
-      </c>
-      <c r="AB196">
-        <v>0</v>
-      </c>
-      <c r="AC196">
-        <v>0</v>
-      </c>
-      <c r="AD196">
-        <v>0</v>
-      </c>
-      <c r="AE196">
-        <v>1498181.4168192</v>
-      </c>
-      <c r="AF196">
-        <v>0</v>
-      </c>
-      <c r="AG196">
-        <v>0</v>
-      </c>
-      <c r="AH196">
-        <v>0</v>
-      </c>
-      <c r="AJ196">
-        <v>0</v>
-      </c>
-      <c r="AK196">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="197" spans="1:37">
-      <c r="A197" s="2">
-        <v>44105</v>
-      </c>
-      <c r="B197">
-        <v>195</v>
-      </c>
-      <c r="C197">
-        <v>1137715.655858824</v>
-      </c>
-      <c r="D197">
-        <v>1138198.442082663</v>
-      </c>
-      <c r="E197">
-        <v>0</v>
-      </c>
-      <c r="F197">
-        <v>0</v>
-      </c>
-      <c r="G197">
-        <v>1136127.261351267</v>
-      </c>
-      <c r="H197">
-        <v>690685.0257366077</v>
-      </c>
-      <c r="I197">
-        <v>24252.2503426687</v>
-      </c>
-      <c r="J197">
-        <v>5105.730586805043</v>
-      </c>
-      <c r="K197">
-        <v>1818.5831808</v>
-      </c>
-      <c r="L197">
-        <v>0</v>
-      </c>
-      <c r="M197">
-        <v>0</v>
-      </c>
-      <c r="N197">
-        <v>0</v>
-      </c>
-      <c r="O197">
-        <v>0</v>
-      </c>
-      <c r="P197">
-        <v>0</v>
-      </c>
-      <c r="Q197">
-        <v>0</v>
-      </c>
-      <c r="R197">
-        <v>0</v>
-      </c>
-      <c r="S197">
-        <v>0</v>
-      </c>
-      <c r="T197">
-        <v>0</v>
-      </c>
-      <c r="U197">
-        <v>0</v>
-      </c>
-      <c r="V197">
-        <v>0</v>
-      </c>
-      <c r="W197">
-        <v>362054.1554679333</v>
-      </c>
-      <c r="X197">
-        <v>0</v>
-      </c>
-      <c r="Y197">
-        <v>0</v>
-      </c>
-      <c r="Z197">
-        <v>0</v>
-      </c>
-      <c r="AA197">
-        <v>0</v>
-      </c>
-      <c r="AB197">
-        <v>0</v>
-      </c>
-      <c r="AC197">
-        <v>0</v>
-      </c>
-      <c r="AD197">
-        <v>0</v>
-      </c>
-      <c r="AE197">
-        <v>1498181.4168192</v>
-      </c>
-      <c r="AF197">
-        <v>0</v>
-      </c>
-      <c r="AG197">
-        <v>0</v>
-      </c>
-      <c r="AH197">
-        <v>0</v>
-      </c>
-      <c r="AJ197">
-        <v>0</v>
-      </c>
-      <c r="AK197">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="198" spans="1:37">
-      <c r="A198" s="2">
-        <v>44106</v>
-      </c>
-      <c r="B198">
-        <v>196</v>
-      </c>
-      <c r="C198">
-        <v>1137715.655858824</v>
-      </c>
-      <c r="D198">
-        <v>1138198.442082663</v>
-      </c>
-      <c r="E198">
-        <v>0</v>
-      </c>
-      <c r="F198">
-        <v>0</v>
-      </c>
-      <c r="G198">
-        <v>1136127.261351267</v>
-      </c>
-      <c r="H198">
-        <v>690685.0257366077</v>
-      </c>
-      <c r="I198">
-        <v>24252.2503426687</v>
-      </c>
-      <c r="J198">
-        <v>5105.730586805043</v>
-      </c>
-      <c r="K198">
-        <v>1818.5831808</v>
-      </c>
-      <c r="L198">
-        <v>0</v>
-      </c>
-      <c r="M198">
-        <v>0</v>
-      </c>
-      <c r="N198">
-        <v>0</v>
-      </c>
-      <c r="O198">
-        <v>0</v>
-      </c>
-      <c r="P198">
-        <v>0</v>
-      </c>
-      <c r="Q198">
-        <v>0</v>
-      </c>
-      <c r="R198">
-        <v>0</v>
-      </c>
-      <c r="S198">
-        <v>0</v>
-      </c>
-      <c r="T198">
-        <v>0</v>
-      </c>
-      <c r="U198">
-        <v>0</v>
-      </c>
-      <c r="V198">
-        <v>0</v>
-      </c>
-      <c r="W198">
-        <v>362054.1554679333</v>
-      </c>
-      <c r="X198">
-        <v>0</v>
-      </c>
-      <c r="Y198">
-        <v>0</v>
-      </c>
-      <c r="Z198">
-        <v>0</v>
-      </c>
-      <c r="AA198">
-        <v>0</v>
-      </c>
-      <c r="AB198">
-        <v>0</v>
-      </c>
-      <c r="AC198">
-        <v>0</v>
-      </c>
-      <c r="AD198">
-        <v>0</v>
-      </c>
-      <c r="AE198">
-        <v>1498181.4168192</v>
-      </c>
-      <c r="AF198">
-        <v>0</v>
-      </c>
-      <c r="AG198">
-        <v>0</v>
-      </c>
-      <c r="AH198">
-        <v>0</v>
-      </c>
-      <c r="AJ198">
-        <v>0</v>
-      </c>
-      <c r="AK198">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="199" spans="1:37">
-      <c r="A199" s="2">
-        <v>44107</v>
-      </c>
-      <c r="B199">
-        <v>197</v>
-      </c>
-      <c r="C199">
-        <v>1137715.655858824</v>
-      </c>
-      <c r="D199">
-        <v>1138198.442082663</v>
-      </c>
-      <c r="E199">
-        <v>0</v>
-      </c>
-      <c r="F199">
-        <v>0</v>
-      </c>
-      <c r="G199">
-        <v>1136127.261351267</v>
-      </c>
-      <c r="H199">
-        <v>690685.0257366077</v>
-      </c>
-      <c r="I199">
-        <v>24252.2503426687</v>
-      </c>
-      <c r="J199">
-        <v>5105.730586805043</v>
-      </c>
-      <c r="K199">
-        <v>1818.5831808</v>
-      </c>
-      <c r="L199">
-        <v>0</v>
-      </c>
-      <c r="M199">
-        <v>0</v>
-      </c>
-      <c r="N199">
-        <v>0</v>
-      </c>
-      <c r="O199">
-        <v>0</v>
-      </c>
-      <c r="P199">
-        <v>0</v>
-      </c>
-      <c r="Q199">
-        <v>0</v>
-      </c>
-      <c r="R199">
-        <v>0</v>
-      </c>
-      <c r="S199">
-        <v>0</v>
-      </c>
-      <c r="T199">
-        <v>0</v>
-      </c>
-      <c r="U199">
-        <v>0</v>
-      </c>
-      <c r="V199">
-        <v>0</v>
-      </c>
-      <c r="W199">
-        <v>362054.1554679333</v>
-      </c>
-      <c r="X199">
-        <v>0</v>
-      </c>
-      <c r="Y199">
-        <v>0</v>
-      </c>
-      <c r="Z199">
-        <v>0</v>
-      </c>
-      <c r="AA199">
-        <v>0</v>
-      </c>
-      <c r="AB199">
-        <v>0</v>
-      </c>
-      <c r="AC199">
-        <v>0</v>
-      </c>
-      <c r="AD199">
-        <v>0</v>
-      </c>
-      <c r="AE199">
-        <v>1498181.4168192</v>
-      </c>
-      <c r="AF199">
-        <v>0</v>
-      </c>
-      <c r="AG199">
-        <v>0</v>
-      </c>
-      <c r="AH199">
-        <v>0</v>
-      </c>
-      <c r="AJ199">
-        <v>0</v>
-      </c>
-      <c r="AK199">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="200" spans="1:37">
-      <c r="A200" s="2">
-        <v>44108</v>
-      </c>
-      <c r="B200">
-        <v>198</v>
-      </c>
-      <c r="C200">
-        <v>1137715.655858824</v>
-      </c>
-      <c r="D200">
-        <v>1138198.442082663</v>
-      </c>
-      <c r="E200">
-        <v>0</v>
-      </c>
-      <c r="F200">
-        <v>0</v>
-      </c>
-      <c r="G200">
-        <v>1136127.261351267</v>
-      </c>
-      <c r="H200">
-        <v>690685.0257366077</v>
-      </c>
-      <c r="I200">
-        <v>24252.2503426687</v>
-      </c>
-      <c r="J200">
-        <v>5105.730586805043</v>
-      </c>
-      <c r="K200">
-        <v>1818.5831808</v>
-      </c>
-      <c r="L200">
-        <v>0</v>
-      </c>
-      <c r="M200">
-        <v>0</v>
-      </c>
-      <c r="N200">
-        <v>0</v>
-      </c>
-      <c r="O200">
-        <v>0</v>
-      </c>
-      <c r="P200">
-        <v>0</v>
-      </c>
-      <c r="Q200">
-        <v>0</v>
-      </c>
-      <c r="R200">
-        <v>0</v>
-      </c>
-      <c r="S200">
-        <v>0</v>
-      </c>
-      <c r="T200">
-        <v>0</v>
-      </c>
-      <c r="U200">
-        <v>0</v>
-      </c>
-      <c r="V200">
-        <v>0</v>
-      </c>
-      <c r="W200">
-        <v>362054.1554679333</v>
-      </c>
-      <c r="X200">
-        <v>0</v>
-      </c>
-      <c r="Y200">
-        <v>0</v>
-      </c>
-      <c r="Z200">
-        <v>0</v>
-      </c>
-      <c r="AA200">
-        <v>0</v>
-      </c>
-      <c r="AB200">
-        <v>0</v>
-      </c>
-      <c r="AC200">
-        <v>0</v>
-      </c>
-      <c r="AD200">
-        <v>0</v>
-      </c>
-      <c r="AE200">
-        <v>1498181.4168192</v>
-      </c>
-      <c r="AF200">
-        <v>0</v>
-      </c>
-      <c r="AG200">
-        <v>0</v>
-      </c>
-      <c r="AH200">
-        <v>0</v>
-      </c>
-      <c r="AJ200">
-        <v>0</v>
-      </c>
-      <c r="AK200">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="201" spans="1:37">
-      <c r="A201" s="2">
-        <v>44109</v>
-      </c>
-      <c r="B201">
-        <v>199</v>
-      </c>
-      <c r="C201">
-        <v>1137715.655858824</v>
-      </c>
-      <c r="D201">
-        <v>1138198.442082663</v>
-      </c>
-      <c r="E201">
-        <v>0</v>
-      </c>
-      <c r="F201">
-        <v>0</v>
-      </c>
-      <c r="G201">
-        <v>1136127.261351267</v>
-      </c>
-      <c r="H201">
-        <v>690685.0257366077</v>
-      </c>
-      <c r="I201">
-        <v>24252.2503426687</v>
-      </c>
-      <c r="J201">
-        <v>5105.730586805043</v>
-      </c>
-      <c r="K201">
-        <v>1818.5831808</v>
-      </c>
-      <c r="L201">
-        <v>0</v>
-      </c>
-      <c r="M201">
-        <v>0</v>
-      </c>
-      <c r="N201">
-        <v>0</v>
-      </c>
-      <c r="O201">
-        <v>0</v>
-      </c>
-      <c r="P201">
-        <v>0</v>
-      </c>
-      <c r="Q201">
-        <v>0</v>
-      </c>
-      <c r="R201">
-        <v>0</v>
-      </c>
-      <c r="S201">
-        <v>0</v>
-      </c>
-      <c r="T201">
-        <v>0</v>
-      </c>
-      <c r="U201">
-        <v>0</v>
-      </c>
-      <c r="V201">
-        <v>0</v>
-      </c>
-      <c r="W201">
-        <v>362054.1554679333</v>
-      </c>
-      <c r="X201">
-        <v>0</v>
-      </c>
-      <c r="Y201">
-        <v>0</v>
-      </c>
-      <c r="Z201">
-        <v>0</v>
-      </c>
-      <c r="AA201">
-        <v>0</v>
-      </c>
-      <c r="AB201">
-        <v>0</v>
-      </c>
-      <c r="AC201">
-        <v>0</v>
-      </c>
-      <c r="AD201">
-        <v>0</v>
-      </c>
-      <c r="AE201">
-        <v>1498181.4168192</v>
-      </c>
-      <c r="AF201">
-        <v>0</v>
-      </c>
-      <c r="AG201">
-        <v>0</v>
-      </c>
-      <c r="AH201">
-        <v>0</v>
-      </c>
-      <c r="AJ201">
-        <v>0</v>
-      </c>
-      <c r="AK201">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="202" spans="1:37">
-      <c r="A202" s="2">
-        <v>44110</v>
-      </c>
-      <c r="B202">
-        <v>200</v>
-      </c>
-      <c r="C202">
-        <v>1137715.655858824</v>
-      </c>
-      <c r="D202">
-        <v>1138198.442082663</v>
-      </c>
-      <c r="E202">
-        <v>0</v>
-      </c>
-      <c r="F202">
-        <v>0</v>
-      </c>
-      <c r="G202">
-        <v>1136127.261351267</v>
-      </c>
-      <c r="H202">
-        <v>690685.0257366077</v>
-      </c>
-      <c r="I202">
-        <v>24252.2503426687</v>
-      </c>
-      <c r="J202">
-        <v>5105.730586805043</v>
-      </c>
-      <c r="K202">
-        <v>1818.5831808</v>
-      </c>
-      <c r="L202">
-        <v>0</v>
-      </c>
-      <c r="M202">
-        <v>0</v>
-      </c>
-      <c r="N202">
-        <v>0</v>
-      </c>
-      <c r="O202">
-        <v>0</v>
-      </c>
-      <c r="P202">
-        <v>0</v>
-      </c>
-      <c r="Q202">
-        <v>0</v>
-      </c>
-      <c r="R202">
-        <v>0</v>
-      </c>
-      <c r="S202">
-        <v>0</v>
-      </c>
-      <c r="T202">
-        <v>0</v>
-      </c>
-      <c r="U202">
-        <v>0</v>
-      </c>
-      <c r="V202">
-        <v>0</v>
-      </c>
-      <c r="W202">
-        <v>362054.1554679333</v>
-      </c>
-      <c r="X202">
-        <v>0</v>
-      </c>
-      <c r="Y202">
-        <v>0</v>
-      </c>
-      <c r="Z202">
-        <v>0</v>
-      </c>
-      <c r="AA202">
-        <v>0</v>
-      </c>
-      <c r="AB202">
-        <v>0</v>
-      </c>
-      <c r="AC202">
-        <v>0</v>
-      </c>
-      <c r="AD202">
-        <v>0</v>
-      </c>
-      <c r="AE202">
-        <v>1498181.4168192</v>
-      </c>
-      <c r="AF202">
-        <v>0</v>
-      </c>
-      <c r="AG202">
-        <v>0</v>
-      </c>
-      <c r="AH202">
-        <v>0</v>
-      </c>
-      <c r="AJ202">
-        <v>0</v>
-      </c>
-      <c r="AK202">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="203" spans="1:37">
-      <c r="A203" s="2">
-        <v>44111</v>
-      </c>
-      <c r="B203">
-        <v>201</v>
-      </c>
-      <c r="C203">
-        <v>1137715.655858824</v>
-      </c>
-      <c r="D203">
-        <v>1138198.442082663</v>
-      </c>
-      <c r="E203">
-        <v>0</v>
-      </c>
-      <c r="F203">
-        <v>0</v>
-      </c>
-      <c r="G203">
-        <v>1136127.261351267</v>
-      </c>
-      <c r="H203">
-        <v>690685.0257366077</v>
-      </c>
-      <c r="I203">
-        <v>24252.2503426687</v>
-      </c>
-      <c r="J203">
-        <v>5105.730586805043</v>
-      </c>
-      <c r="K203">
-        <v>1818.5831808</v>
-      </c>
-      <c r="L203">
-        <v>0</v>
-      </c>
-      <c r="M203">
-        <v>0</v>
-      </c>
-      <c r="N203">
-        <v>0</v>
-      </c>
-      <c r="O203">
-        <v>0</v>
-      </c>
-      <c r="P203">
-        <v>0</v>
-      </c>
-      <c r="Q203">
-        <v>0</v>
-      </c>
-      <c r="R203">
-        <v>0</v>
-      </c>
-      <c r="S203">
-        <v>0</v>
-      </c>
-      <c r="T203">
-        <v>0</v>
-      </c>
-      <c r="U203">
-        <v>0</v>
-      </c>
-      <c r="V203">
-        <v>0</v>
-      </c>
-      <c r="W203">
-        <v>362054.1554679333</v>
-      </c>
-      <c r="X203">
-        <v>0</v>
-      </c>
-      <c r="Y203">
-        <v>0</v>
-      </c>
-      <c r="Z203">
-        <v>0</v>
-      </c>
-      <c r="AA203">
-        <v>0</v>
-      </c>
-      <c r="AB203">
-        <v>0</v>
-      </c>
-      <c r="AC203">
-        <v>0</v>
-      </c>
-      <c r="AD203">
-        <v>0</v>
-      </c>
-      <c r="AE203">
-        <v>1498181.4168192</v>
-      </c>
-      <c r="AF203">
-        <v>0</v>
-      </c>
-      <c r="AG203">
-        <v>0</v>
-      </c>
-      <c r="AH203">
-        <v>0</v>
-      </c>
-      <c r="AJ203">
-        <v>0</v>
-      </c>
-      <c r="AK203">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="204" spans="1:37">
-      <c r="A204" s="2">
-        <v>44112</v>
-      </c>
-      <c r="B204">
-        <v>202</v>
-      </c>
-      <c r="C204">
-        <v>1137715.655858824</v>
-      </c>
-      <c r="D204">
-        <v>1138198.442082663</v>
-      </c>
-      <c r="E204">
-        <v>0</v>
-      </c>
-      <c r="F204">
-        <v>0</v>
-      </c>
-      <c r="G204">
-        <v>1136127.261351267</v>
-      </c>
-      <c r="H204">
-        <v>690685.0257366077</v>
-      </c>
-      <c r="I204">
-        <v>24252.2503426687</v>
-      </c>
-      <c r="J204">
-        <v>5105.730586805043</v>
-      </c>
-      <c r="K204">
-        <v>1818.5831808</v>
-      </c>
-      <c r="L204">
-        <v>0</v>
-      </c>
-      <c r="M204">
-        <v>0</v>
-      </c>
-      <c r="N204">
-        <v>0</v>
-      </c>
-      <c r="O204">
-        <v>0</v>
-      </c>
-      <c r="P204">
-        <v>0</v>
-      </c>
-      <c r="Q204">
-        <v>0</v>
-      </c>
-      <c r="R204">
-        <v>0</v>
-      </c>
-      <c r="S204">
-        <v>0</v>
-      </c>
-      <c r="T204">
-        <v>0</v>
-      </c>
-      <c r="U204">
-        <v>0</v>
-      </c>
-      <c r="V204">
-        <v>0</v>
-      </c>
-      <c r="W204">
-        <v>362054.1554679333</v>
-      </c>
-      <c r="X204">
-        <v>0</v>
-      </c>
-      <c r="Y204">
-        <v>0</v>
-      </c>
-      <c r="Z204">
-        <v>0</v>
-      </c>
-      <c r="AA204">
-        <v>0</v>
-      </c>
-      <c r="AB204">
-        <v>0</v>
-      </c>
-      <c r="AC204">
-        <v>0</v>
-      </c>
-      <c r="AD204">
-        <v>0</v>
-      </c>
-      <c r="AE204">
-        <v>1498181.4168192</v>
-      </c>
-      <c r="AF204">
-        <v>0</v>
-      </c>
-      <c r="AG204">
-        <v>0</v>
-      </c>
-      <c r="AH204">
-        <v>0</v>
-      </c>
-      <c r="AJ204">
-        <v>0</v>
-      </c>
-      <c r="AK204">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="205" spans="1:37">
-      <c r="A205" s="2">
-        <v>44113</v>
-      </c>
-      <c r="B205">
-        <v>203</v>
-      </c>
-      <c r="C205">
-        <v>1137715.655858824</v>
-      </c>
-      <c r="D205">
-        <v>1138198.442082663</v>
-      </c>
-      <c r="E205">
-        <v>0</v>
-      </c>
-      <c r="F205">
-        <v>0</v>
-      </c>
-      <c r="G205">
-        <v>1136127.261351267</v>
-      </c>
-      <c r="H205">
-        <v>690685.0257366077</v>
-      </c>
-      <c r="I205">
-        <v>24252.2503426687</v>
-      </c>
-      <c r="J205">
-        <v>5105.730586805043</v>
-      </c>
-      <c r="K205">
-        <v>1818.5831808</v>
-      </c>
-      <c r="L205">
-        <v>0</v>
-      </c>
-      <c r="M205">
-        <v>0</v>
-      </c>
-      <c r="N205">
-        <v>0</v>
-      </c>
-      <c r="O205">
-        <v>0</v>
-      </c>
-      <c r="P205">
-        <v>0</v>
-      </c>
-      <c r="Q205">
-        <v>0</v>
-      </c>
-      <c r="R205">
-        <v>0</v>
-      </c>
-      <c r="S205">
-        <v>0</v>
-      </c>
-      <c r="T205">
-        <v>0</v>
-      </c>
-      <c r="U205">
-        <v>0</v>
-      </c>
-      <c r="V205">
-        <v>0</v>
-      </c>
-      <c r="W205">
-        <v>362054.1554679333</v>
-      </c>
-      <c r="X205">
-        <v>0</v>
-      </c>
-      <c r="Y205">
-        <v>0</v>
-      </c>
-      <c r="Z205">
-        <v>0</v>
-      </c>
-      <c r="AA205">
-        <v>0</v>
-      </c>
-      <c r="AB205">
-        <v>0</v>
-      </c>
-      <c r="AC205">
-        <v>0</v>
-      </c>
-      <c r="AD205">
-        <v>0</v>
-      </c>
-      <c r="AE205">
-        <v>1498181.4168192</v>
-      </c>
-      <c r="AF205">
-        <v>0</v>
-      </c>
-      <c r="AG205">
-        <v>0</v>
-      </c>
-      <c r="AH205">
-        <v>0</v>
-      </c>
-      <c r="AJ205">
-        <v>0</v>
-      </c>
-      <c r="AK205">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="206" spans="1:37">
-      <c r="A206" s="2">
-        <v>44114</v>
-      </c>
-      <c r="B206">
-        <v>204</v>
-      </c>
-      <c r="C206">
-        <v>1137715.655858824</v>
-      </c>
-      <c r="D206">
-        <v>1138198.442082663</v>
-      </c>
-      <c r="E206">
-        <v>0</v>
-      </c>
-      <c r="F206">
-        <v>0</v>
-      </c>
-      <c r="G206">
-        <v>1136127.261351267</v>
-      </c>
-      <c r="H206">
-        <v>690685.0257366077</v>
-      </c>
-      <c r="I206">
-        <v>24252.2503426687</v>
-      </c>
-      <c r="J206">
-        <v>5105.730586805043</v>
-      </c>
-      <c r="K206">
-        <v>1818.5831808</v>
-      </c>
-      <c r="L206">
-        <v>0</v>
-      </c>
-      <c r="M206">
-        <v>0</v>
-      </c>
-      <c r="N206">
-        <v>0</v>
-      </c>
-      <c r="O206">
-        <v>0</v>
-      </c>
-      <c r="P206">
-        <v>0</v>
-      </c>
-      <c r="Q206">
-        <v>0</v>
-      </c>
-      <c r="R206">
-        <v>0</v>
-      </c>
-      <c r="S206">
-        <v>0</v>
-      </c>
-      <c r="T206">
-        <v>0</v>
-      </c>
-      <c r="U206">
-        <v>0</v>
-      </c>
-      <c r="V206">
-        <v>0</v>
-      </c>
-      <c r="W206">
-        <v>362054.1554679333</v>
-      </c>
-      <c r="X206">
-        <v>0</v>
-      </c>
-      <c r="Y206">
-        <v>0</v>
-      </c>
-      <c r="Z206">
-        <v>0</v>
-      </c>
-      <c r="AA206">
-        <v>0</v>
-      </c>
-      <c r="AB206">
-        <v>0</v>
-      </c>
-      <c r="AC206">
-        <v>0</v>
-      </c>
-      <c r="AD206">
-        <v>0</v>
-      </c>
-      <c r="AE206">
-        <v>1498181.4168192</v>
-      </c>
-      <c r="AF206">
-        <v>0</v>
-      </c>
-      <c r="AG206">
-        <v>0</v>
-      </c>
-      <c r="AH206">
-        <v>0</v>
-      </c>
-      <c r="AJ206">
-        <v>0</v>
-      </c>
-      <c r="AK206">
         <v>0</v>
       </c>
     </row>
@@ -24023,7 +19733,7 @@
         <v>44</v>
       </c>
       <c r="B7" s="3">
-        <v>44114</v>
+        <v>44075</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -24031,7 +19741,7 @@
         <v>45</v>
       </c>
       <c r="B8">
-        <v>204</v>
+        <v>165</v>
       </c>
     </row>
     <row r="9" spans="1:2">

</xml_diff>